<commit_message>
modified excel and put in new tsv file
</commit_message>
<xml_diff>
--- a/Survey Data.xlsx
+++ b/Survey Data.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuzhenliu/Desktop/tfcb-homework01/tfcb-homework01/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ECBABD6-311D-AF40-94AD-4B7E762CF268}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC188A02-CE6A-1D40-9E1A-4C2522678A13}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="460" windowWidth="16300" windowHeight="14760" tabRatio="481" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="320" yWindow="460" windowWidth="16300" windowHeight="14760" tabRatio="481" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2013" sheetId="1" r:id="rId1"/>
     <sheet name="2014" sheetId="2" r:id="rId2"/>
-    <sheet name="2013_cleaned" sheetId="3" r:id="rId3"/>
-    <sheet name="2014_cleaned" sheetId="4" r:id="rId4"/>
+    <sheet name="cleaned" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="43">
   <si>
     <t>NA</t>
   </si>
@@ -757,7 +756,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -801,7 +800,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -2316,10 +2315,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA73557D-4CC3-4240-B18F-BDC5510655DB}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2764,476 +2763,21 @@
         <v>40</v>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4532252-FA9B-7C47-A35E-F11424E0A9A6}">
-  <dimension ref="A1:F28"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="22">
-        <v>41648</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>40</v>
-      </c>
-      <c r="F2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="22">
-        <v>41648</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3">
-        <v>36</v>
-      </c>
-      <c r="F3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="22">
-        <v>41711</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4">
-        <v>51</v>
-      </c>
-      <c r="F4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="22">
-        <v>41711</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5">
-        <v>44</v>
-      </c>
-      <c r="F5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="22">
-        <v>41711</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6">
-        <v>146</v>
-      </c>
-      <c r="F6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="22">
-        <v>41647</v>
-      </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-      <c r="D7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E7" t="s">
-        <v>39</v>
-      </c>
-      <c r="F7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="22">
-        <v>41647</v>
-      </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-      <c r="D8" t="s">
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <v>44</v>
-      </c>
-      <c r="F8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="22">
-        <v>41647</v>
-      </c>
-      <c r="C9">
-        <v>2</v>
-      </c>
-      <c r="D9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E9">
-        <v>7</v>
-      </c>
-      <c r="F9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="22">
-        <v>41647</v>
-      </c>
-      <c r="C10">
-        <v>2</v>
-      </c>
-      <c r="D10" t="s">
-        <v>1</v>
-      </c>
-      <c r="E10">
-        <v>45</v>
-      </c>
-      <c r="F10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="22">
-        <v>41647</v>
-      </c>
-      <c r="C11">
-        <v>2</v>
-      </c>
-      <c r="D11" t="s">
-        <v>39</v>
-      </c>
-      <c r="E11" t="s">
-        <v>39</v>
-      </c>
-      <c r="F11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" s="22">
-        <v>41647</v>
-      </c>
-      <c r="C12">
-        <v>2</v>
-      </c>
-      <c r="D12" t="s">
-        <v>1</v>
-      </c>
-      <c r="E12">
-        <v>157</v>
-      </c>
-      <c r="F12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="22">
-        <v>41647</v>
-      </c>
-      <c r="C13">
-        <v>2</v>
-      </c>
-      <c r="D13" t="s">
-        <v>39</v>
-      </c>
-      <c r="E13" t="s">
-        <v>39</v>
-      </c>
-      <c r="F13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B14" s="22">
-        <v>41688</v>
-      </c>
-      <c r="C14">
-        <v>2</v>
-      </c>
-      <c r="D14" t="s">
-        <v>1</v>
-      </c>
-      <c r="E14">
-        <v>218</v>
-      </c>
-      <c r="F14" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="22">
-        <v>41688</v>
-      </c>
-      <c r="C15">
-        <v>2</v>
-      </c>
-      <c r="D15" t="s">
-        <v>3</v>
-      </c>
-      <c r="E15">
-        <v>7</v>
-      </c>
-      <c r="F15" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A16" t="s">
-        <v>2</v>
-      </c>
-      <c r="B16" s="22">
-        <v>41688</v>
-      </c>
-      <c r="C16">
-        <v>2</v>
-      </c>
-      <c r="D16" t="s">
-        <v>1</v>
-      </c>
-      <c r="E16">
-        <v>52</v>
-      </c>
-      <c r="F16" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A17" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" s="22">
-        <v>42074</v>
-      </c>
-      <c r="C17">
-        <v>3</v>
-      </c>
-      <c r="D17" t="s">
-        <v>1</v>
-      </c>
-      <c r="E17">
-        <v>8</v>
-      </c>
-      <c r="F17" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A18" t="s">
-        <v>0</v>
-      </c>
-      <c r="B18" s="22">
-        <v>42102</v>
-      </c>
-      <c r="C18">
-        <v>3</v>
-      </c>
-      <c r="D18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E18" t="s">
-        <v>39</v>
-      </c>
-      <c r="F18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A19" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" s="22">
-        <v>42130</v>
-      </c>
-      <c r="C19">
-        <v>3</v>
-      </c>
-      <c r="D19" t="s">
-        <v>39</v>
-      </c>
-      <c r="E19" t="s">
-        <v>39</v>
-      </c>
-      <c r="F19" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A20" t="s">
-        <v>0</v>
-      </c>
-      <c r="B20" s="22">
-        <v>42142</v>
-      </c>
-      <c r="C20">
-        <v>3</v>
-      </c>
-      <c r="D20" t="s">
-        <v>3</v>
-      </c>
-      <c r="E20">
-        <v>182</v>
-      </c>
-      <c r="F20" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A21" t="s">
-        <v>6</v>
-      </c>
-      <c r="B21" s="22">
-        <v>42164</v>
-      </c>
-      <c r="C21">
-        <v>3</v>
-      </c>
-      <c r="D21" t="s">
-        <v>3</v>
-      </c>
-      <c r="E21">
-        <v>29</v>
-      </c>
-      <c r="F21" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A22" t="s">
-        <v>0</v>
-      </c>
-      <c r="B22" s="22">
-        <v>42193</v>
-      </c>
-      <c r="C22">
-        <v>3</v>
-      </c>
-      <c r="D22" t="s">
-        <v>3</v>
-      </c>
-      <c r="E22">
-        <v>115</v>
-      </c>
-      <c r="F22" t="s">
-        <v>40</v>
-      </c>
-    </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B23" s="22">
-        <v>42193</v>
+        <v>41648</v>
       </c>
       <c r="C23">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D23" t="s">
         <v>1</v>
       </c>
       <c r="E23">
-        <v>190</v>
+        <v>40</v>
       </c>
       <c r="F23" t="s">
         <v>40</v>
@@ -3244,16 +2788,16 @@
         <v>2</v>
       </c>
       <c r="B24" s="22">
-        <v>28498</v>
+        <v>41648</v>
       </c>
       <c r="C24">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D24" t="s">
         <v>3</v>
       </c>
       <c r="E24">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F24" t="s">
         <v>40</v>
@@ -3264,19 +2808,19 @@
         <v>2</v>
       </c>
       <c r="B25" s="22">
-        <v>28498</v>
+        <v>41711</v>
       </c>
       <c r="C25">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>1</v>
-      </c>
-      <c r="E25" t="s">
-        <v>39</v>
+        <v>3</v>
+      </c>
+      <c r="E25">
+        <v>51</v>
       </c>
       <c r="F25" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.15">
@@ -3284,16 +2828,16 @@
         <v>2</v>
       </c>
       <c r="B26" s="22">
-        <v>28498</v>
+        <v>41711</v>
       </c>
       <c r="C26">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D26" t="s">
         <v>3</v>
       </c>
       <c r="E26">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F26" t="s">
         <v>40</v>
@@ -3301,19 +2845,19 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>41</v>
+        <v>5</v>
       </c>
       <c r="B27" s="22">
-        <v>28498</v>
+        <v>41711</v>
       </c>
       <c r="C27">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D27" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E27">
-        <v>52</v>
+        <v>146</v>
       </c>
       <c r="F27" t="s">
         <v>40</v>
@@ -3321,21 +2865,441 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" s="22">
+        <v>41647</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28" t="s">
+        <v>39</v>
+      </c>
+      <c r="E28" t="s">
+        <v>39</v>
+      </c>
+      <c r="F28" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A29" t="s">
+        <v>2</v>
+      </c>
+      <c r="B29" s="22">
+        <v>41647</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29" t="s">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>44</v>
+      </c>
+      <c r="F29" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" s="22">
+        <v>41647</v>
+      </c>
+      <c r="C30">
+        <v>2</v>
+      </c>
+      <c r="D30" t="s">
+        <v>3</v>
+      </c>
+      <c r="E30">
+        <v>7</v>
+      </c>
+      <c r="F30" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A31" t="s">
+        <v>2</v>
+      </c>
+      <c r="B31" s="22">
+        <v>41647</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="D31" t="s">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>45</v>
+      </c>
+      <c r="F31" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A32" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" s="22">
+        <v>41647</v>
+      </c>
+      <c r="C32">
+        <v>2</v>
+      </c>
+      <c r="D32" t="s">
+        <v>39</v>
+      </c>
+      <c r="E32" t="s">
+        <v>39</v>
+      </c>
+      <c r="F32" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A33" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" s="22">
+        <v>41647</v>
+      </c>
+      <c r="C33">
+        <v>2</v>
+      </c>
+      <c r="D33" t="s">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>157</v>
+      </c>
+      <c r="F33" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A34" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34" s="22">
+        <v>41647</v>
+      </c>
+      <c r="C34">
+        <v>2</v>
+      </c>
+      <c r="D34" t="s">
+        <v>39</v>
+      </c>
+      <c r="E34" t="s">
+        <v>39</v>
+      </c>
+      <c r="F34" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B35" s="22">
+        <v>41688</v>
+      </c>
+      <c r="C35">
+        <v>2</v>
+      </c>
+      <c r="D35" t="s">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <v>218</v>
+      </c>
+      <c r="F35" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A36" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36" s="22">
+        <v>41688</v>
+      </c>
+      <c r="C36">
+        <v>2</v>
+      </c>
+      <c r="D36" t="s">
+        <v>3</v>
+      </c>
+      <c r="E36">
+        <v>7</v>
+      </c>
+      <c r="F36" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A37" t="s">
+        <v>2</v>
+      </c>
+      <c r="B37" s="22">
+        <v>41688</v>
+      </c>
+      <c r="C37">
+        <v>2</v>
+      </c>
+      <c r="D37" t="s">
+        <v>1</v>
+      </c>
+      <c r="E37">
+        <v>52</v>
+      </c>
+      <c r="F37" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A38" t="s">
+        <v>4</v>
+      </c>
+      <c r="B38" s="22">
+        <v>42074</v>
+      </c>
+      <c r="C38">
+        <v>3</v>
+      </c>
+      <c r="D38" t="s">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <v>8</v>
+      </c>
+      <c r="F38" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A39" t="s">
+        <v>0</v>
+      </c>
+      <c r="B39" s="22">
+        <v>42102</v>
+      </c>
+      <c r="C39">
+        <v>3</v>
+      </c>
+      <c r="D39" t="s">
+        <v>3</v>
+      </c>
+      <c r="E39" t="s">
+        <v>39</v>
+      </c>
+      <c r="F39" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A40" t="s">
+        <v>39</v>
+      </c>
+      <c r="B40" s="22">
+        <v>42130</v>
+      </c>
+      <c r="C40">
+        <v>3</v>
+      </c>
+      <c r="D40" t="s">
+        <v>39</v>
+      </c>
+      <c r="E40" t="s">
+        <v>39</v>
+      </c>
+      <c r="F40" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A41" t="s">
+        <v>0</v>
+      </c>
+      <c r="B41" s="22">
+        <v>42142</v>
+      </c>
+      <c r="C41">
+        <v>3</v>
+      </c>
+      <c r="D41" t="s">
+        <v>3</v>
+      </c>
+      <c r="E41">
+        <v>182</v>
+      </c>
+      <c r="F41" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A42" t="s">
+        <v>6</v>
+      </c>
+      <c r="B42" s="22">
+        <v>42164</v>
+      </c>
+      <c r="C42">
+        <v>3</v>
+      </c>
+      <c r="D42" t="s">
+        <v>3</v>
+      </c>
+      <c r="E42">
+        <v>29</v>
+      </c>
+      <c r="F42" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A43" t="s">
+        <v>0</v>
+      </c>
+      <c r="B43" s="22">
+        <v>42193</v>
+      </c>
+      <c r="C43">
+        <v>3</v>
+      </c>
+      <c r="D43" t="s">
+        <v>3</v>
+      </c>
+      <c r="E43">
+        <v>115</v>
+      </c>
+      <c r="F43" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A44" t="s">
+        <v>0</v>
+      </c>
+      <c r="B44" s="22">
+        <v>42193</v>
+      </c>
+      <c r="C44">
+        <v>3</v>
+      </c>
+      <c r="D44" t="s">
+        <v>1</v>
+      </c>
+      <c r="E44">
+        <v>190</v>
+      </c>
+      <c r="F44" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A45" t="s">
+        <v>2</v>
+      </c>
+      <c r="B45" s="22">
+        <v>28498</v>
+      </c>
+      <c r="C45">
+        <v>4</v>
+      </c>
+      <c r="D45" t="s">
+        <v>3</v>
+      </c>
+      <c r="E45">
+        <v>37</v>
+      </c>
+      <c r="F45" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A46" t="s">
+        <v>2</v>
+      </c>
+      <c r="B46" s="22">
+        <v>28498</v>
+      </c>
+      <c r="C46">
+        <v>4</v>
+      </c>
+      <c r="D46" t="s">
+        <v>1</v>
+      </c>
+      <c r="E46" t="s">
+        <v>39</v>
+      </c>
+      <c r="F46" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A47" t="s">
+        <v>2</v>
+      </c>
+      <c r="B47" s="22">
+        <v>28498</v>
+      </c>
+      <c r="C47">
+        <v>4</v>
+      </c>
+      <c r="D47" t="s">
+        <v>3</v>
+      </c>
+      <c r="E47">
+        <v>48</v>
+      </c>
+      <c r="F47" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A48" t="s">
+        <v>41</v>
+      </c>
+      <c r="B48" s="22">
+        <v>28498</v>
+      </c>
+      <c r="C48">
+        <v>4</v>
+      </c>
+      <c r="D48" t="s">
+        <v>1</v>
+      </c>
+      <c r="E48">
+        <v>52</v>
+      </c>
+      <c r="F48" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A49" t="s">
         <v>42</v>
       </c>
-      <c r="B28" s="22">
+      <c r="B49" s="22">
         <v>28498</v>
       </c>
-      <c r="C28">
+      <c r="C49">
         <v>4</v>
       </c>
-      <c r="D28" t="s">
-        <v>1</v>
-      </c>
-      <c r="E28">
+      <c r="D49" t="s">
+        <v>1</v>
+      </c>
+      <c r="E49">
         <v>35</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F49" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>